<commit_message>
Use https map sources when possible to avoid cross-site warnings.
</commit_message>
<xml_diff>
--- a/application/trunk/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
+++ b/application/trunk/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="9740" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="5060" yWindow="2160" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,72 +174,9 @@
     <t>Stamen Watercolor</t>
   </si>
   <si>
-    <t>http://{s}.tile.openstreetmap.org/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/World_Physical_Map/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/NatGeo_World_Map/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/World_Shaded_Relief/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/Ocean_Basemap/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/World_Terrain_Base/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/World_Topo_Map/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/Specialty/DeLorme_World_Base_Map/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://server.arcgisonline.com/ArcGIS/rest/services/World_Imagery/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://services.arcgisonline.com/ArcGIS/rest/services/Demographics/USA_Tapestry/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.openweathermap.org/map/clouds/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.openweathermap.org/map/rain_cls/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.openweathermap.org/map/temp/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>http://oatile{s}.mqcdn.com/tiles/1.0.0/sat/{z}/{x}/{y}.jpg</t>
   </si>
   <si>
-    <t>http://{s}.tile.stamen.com/toner/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/toner-lite/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/toner-hybrid/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/toner-lines/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/toner-labels/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/terrain/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://{s}.tile.stamen.com/terrain-background/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
-    <t>http://tile.stamen.com/watercolor/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>Tiles &amp;copy; Esri &amp;mdash; Source: US National Park Service</t>
   </si>
   <si>
@@ -273,9 +210,6 @@
     <t>Open Weather Map / Rain</t>
   </si>
   <si>
-    <t>http://{s}.tile.openweathermap.org/map/rain/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>Map data &amp;copy; &lt;a href="http://openweathermap.org"&gt;OpenWeatherMap&lt;/a&gt;</t>
   </si>
   <si>
@@ -288,18 +222,12 @@
     <t>Open Weather Map / Pressure Contour</t>
   </si>
   <si>
-    <t>http://{s}.tile.openweathermap.org/map/pressure_cntr/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>NATIONAL_MAP</t>
   </si>
   <si>
     <t>National Map (US)</t>
   </si>
   <si>
-    <t>http://basemap.nationalmap.gov/ArcGIS/rest/services/USGSTopo/MapServer/tile/{z}/{y}/{x}</t>
-  </si>
-  <si>
     <t>&lt;a href='http:usgs.gov'&gt;USGS&lt;/a&gt; National Map Data</t>
   </si>
   <si>
@@ -318,9 +246,6 @@
     <t>http://gis.srh.noaa.gov/arcgis/services/NDFDTemps/MapServer/WMSServer</t>
   </si>
   <si>
-    <t>http://nowcoast.noaa.gov/wms/com.esri.wms.Esrimap/obs</t>
-  </si>
-  <si>
     <t>NOAA_TEMPERATURE</t>
   </si>
   <si>
@@ -348,9 +273,6 @@
     <t>OpenStreetMap / Black &amp; White</t>
   </si>
   <si>
-    <t>http://{s}.www.toolserver.org/tiles/bw-mapnik/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>Map data &amp;copy; &lt;a href="http://openstreetmap.org"&gt;OpenStreetMap&lt;/a&gt; Contributors</t>
   </si>
   <si>
@@ -360,9 +282,6 @@
     <t>OpenCycleMap</t>
   </si>
   <si>
-    <t>http://{s}.tile.thunderforest.com/cycle/{z}/{x}/{y}.png</t>
-  </si>
-  <si>
     <t>Map data &amp;copy; &lt;a href="http://openstreetmap.org"&gt;OpenStreetMap&lt;/a&gt; Contributors &amp; &lt;a href="http://thunderforest.com/"&gt;Thunderforest&lt;/a&gt;</t>
   </si>
   <si>
@@ -412,6 +331,87 @@
   </si>
   <si>
     <t>THUNDERFOREST_LANDSCAPE</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openstreetmap.org/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.www.toolserver.org/tiles/bw-mapnik/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.thunderforest.com/cycle/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/World_Physical_Map/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/NatGeo_World_Map/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/World_Shaded_Relief/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/Ocean_Basemap/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/World_Terrain_Base/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/World_Topo_Map/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/Specialty/DeLorme_World_Base_Map/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://server.arcgisonline.com/ArcGIS/rest/services/World_Imagery/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://services.arcgisonline.com/ArcGIS/rest/services/Demographics/USA_Tapestry/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openweathermap.org/map/clouds/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openweathermap.org/map/rain/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openweathermap.org/map/rain_cls/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openweathermap.org/map/temp/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://{s}.tile.openweathermap.org/map/pressure_cntr/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://basemap.nationalmap.gov/ArcGIS/rest/services/USGSTopo/MapServer/tile/{z}/{y}/{x}</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/toner/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/toner-lite/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/toner-hybrid/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/toner-lines/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/toner-labels/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/terrain/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/terrain-background/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>https://stamen-tiles-{s}.a.ssl.fastly.net/watercolor/{z}/{x}/{y}.png</t>
+  </si>
+  <si>
+    <t>http://nowcoast.noaa.gov/arcgis/services/nowcoast/analysis_meteohydro_sfc_qpe_time/MapServer/WmsServer</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -496,8 +496,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -513,8 +514,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -529,6 +531,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -860,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -891,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -909,16 +912,16 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>0</v>
@@ -938,10 +941,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="G2">
         <v>18</v>
@@ -952,43 +955,43 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="G3">
         <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G4" s="2">
         <v>18</v>
@@ -1000,25 +1003,25 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G5" s="2">
         <v>18</v>
@@ -1030,25 +1033,25 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G6" s="2">
         <v>18</v>
@@ -1060,25 +1063,25 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G7" s="2">
         <v>18</v>
@@ -1090,7 +1093,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1104,10 +1107,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -1127,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="G9">
         <v>16</v>
@@ -1150,10 +1153,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="G10">
         <v>13</v>
@@ -1173,10 +1176,10 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="G11">
         <v>16</v>
@@ -1196,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="G12">
         <v>13</v>
@@ -1219,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="N13" t="s">
         <v>13</v>
@@ -1239,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -1262,10 +1265,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="N15" t="s">
         <v>15</v>
@@ -1282,10 +1285,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="H16">
         <v>0.25</v>
@@ -1302,10 +1305,10 @@
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H17">
         <v>0.5</v>
@@ -1316,22 +1319,22 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H18">
         <v>0.5</v>
       </c>
       <c r="N18" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1342,10 +1345,10 @@
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H19">
         <v>0.5</v>
@@ -1364,10 +1367,10 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2">
@@ -1384,27 +1387,27 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H21">
         <v>0.25</v>
       </c>
       <c r="N21" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
@@ -1413,10 +1416,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="G22">
         <v>18</v>
@@ -1425,24 +1428,24 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="G23">
         <v>18</v>
@@ -1451,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="60">
@@ -1465,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G24">
         <v>20</v>
@@ -1488,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G25">
         <v>20</v>
@@ -1508,10 +1511,10 @@
         <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G26">
         <v>20</v>
@@ -1528,10 +1531,10 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G27">
         <v>20</v>
@@ -1548,10 +1551,10 @@
         <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G28">
         <v>20</v>
@@ -1571,10 +1574,10 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G29">
         <v>20</v>
@@ -1594,10 +1597,10 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G30">
         <v>20</v>
@@ -1616,11 +1619,11 @@
       <c r="C31" t="b">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>72</v>
+      <c r="E31" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G31">
         <v>16</v>
@@ -1631,39 +1634,39 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="G32">
         <v>18</v>
       </c>
       <c r="N32" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="H33">
         <v>0.25</v>
@@ -1675,27 +1678,27 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="M33">
         <v>16</v>
       </c>
       <c r="N33" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="H34">
         <v>0.25</v>
@@ -1707,16 +1710,19 @@
         <v>1</v>
       </c>
       <c r="L34" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="M34" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="N34" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E31" r:id="rId1" display="https://tile.stamen.com/watercolor/{z}/{x}/{y}.png"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>